<commit_message>
bibliyor excel file loading
</commit_message>
<xml_diff>
--- a/src/main/resources/slr/scopus.xlsx
+++ b/src/main/resources/slr/scopus.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliyamuc/Code/datascope-backend/src/main/resources/biblio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliyamuc/Code/bibliyor/src/main/resources/slr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE4A3D4-AF15-634E-8DC8-C802A94503D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C60C4DF-0FCF-D647-9BAD-D1EBCDDDED67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="500" windowWidth="37080" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="big  data" sheetId="1" r:id="rId1"/>
+    <sheet name="big data" sheetId="1" r:id="rId1"/>
     <sheet name="machine learning" sheetId="2" r:id="rId2"/>
     <sheet name="statistics" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'big  data'!$A$1:$T$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'big data'!$A$1:$T$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'machine learning'!$A$1:$T$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -3694,13 +3694,13 @@
   </sheetPr>
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="125" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScale="125" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="113" style="1" customWidth="1"/>
@@ -3718,7 +3718,7 @@
     <col min="16" max="16" width="14.83203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="15.5" style="1" customWidth="1"/>
     <col min="18" max="18" width="46.1640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="7.1640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.1640625" style="1" customWidth="1"/>
     <col min="20" max="20" width="17" style="1" customWidth="1"/>
     <col min="21" max="21" width="8.33203125" style="1" customWidth="1"/>
     <col min="22" max="16384" width="8.33203125" style="1"/>
@@ -9557,7 +9557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07D1324-951E-0E4D-BCC9-16367D2DB9D9}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
+    <sheetView zoomScale="157" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>